<commit_message>
chore: Se modifican documentos
</commit_message>
<xml_diff>
--- a/3- Desarrollo/04- Inventario Software Y Hardware/01- Sotfware_Kyukeisho.xlsx
+++ b/3- Desarrollo/04- Inventario Software Y Hardware/01- Sotfware_Kyukeisho.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\1803170 - G3\Proyecto_Formativo\Kyukeisho_New\3- Desarrollo\04- Inventario Software Y Hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B7403D2-D5EA-4A91-AF67-B0538134712A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14365EBF-A20A-4027-A608-CCFDB3D7121F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -570,77 +570,31 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -656,37 +610,40 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="6" fontId="3" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="6" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="6" fontId="3" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="165" fontId="10" fillId="4" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="165" fontId="10" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="165" fontId="10" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="6" fontId="3" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="6" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="6" fontId="3" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -701,15 +658,58 @@
     <xf numFmtId="165" fontId="3" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -733,7 +733,7 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>962025</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
@@ -968,83 +968,97 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="B1:AC26"/>
+  <dimension ref="A1:AC26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R7" workbookViewId="0">
-      <selection activeCell="Z25" sqref="Z25:AC25"/>
+    <sheetView tabSelected="1" topLeftCell="M4" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="15" max="15" width="155.85546875" customWidth="1"/>
+    <col min="10" max="10" width="78.85546875" customWidth="1"/>
+    <col min="11" max="11" width="35.28515625" customWidth="1"/>
+    <col min="14" max="14" width="67.7109375" customWidth="1"/>
+    <col min="15" max="15" width="14.42578125" customWidth="1"/>
+    <col min="16" max="16" width="0.42578125" customWidth="1"/>
+    <col min="17" max="17" width="14.42578125" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="0.140625" hidden="1" customWidth="1"/>
+    <col min="19" max="20" width="14.42578125" hidden="1" customWidth="1"/>
+    <col min="22" max="22" width="0.140625" customWidth="1"/>
+    <col min="23" max="24" width="14.42578125" hidden="1" customWidth="1"/>
+    <col min="25" max="25" width="14.42578125" customWidth="1"/>
+    <col min="26" max="26" width="14.42578125" hidden="1" customWidth="1"/>
+    <col min="27" max="27" width="3.85546875" customWidth="1"/>
+    <col min="28" max="28" width="0.140625" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:29" ht="15.75" customHeight="1">
-      <c r="B1" s="11"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="13"/>
+    <row r="1" spans="1:28" ht="15.75" customHeight="1">
+      <c r="A1" s="64"/>
+      <c r="B1" s="65"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="1"/>
       <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="36"/>
-      <c r="X1" s="2"/>
-      <c r="Y1" s="5" t="s">
+      <c r="G1" s="4"/>
+      <c r="W1" s="2"/>
+      <c r="X1" s="62" t="s">
         <v>0</v>
       </c>
+      <c r="Y1" s="6"/>
       <c r="Z1" s="6"/>
-      <c r="AA1" s="6"/>
-      <c r="AB1" s="7"/>
-      <c r="AC1" s="1"/>
-    </row>
-    <row r="2" spans="2:29" ht="15.75" customHeight="1">
-      <c r="B2" s="14"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="15"/>
+      <c r="AA1" s="7"/>
+      <c r="AB1" s="1"/>
+    </row>
+    <row r="2" spans="1:28" ht="15.75" customHeight="1">
+      <c r="A2" s="67"/>
+      <c r="B2" s="68"/>
+      <c r="C2" s="68"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="1"/>
       <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="X2" s="2"/>
-      <c r="Y2" s="8" t="s">
+      <c r="W2" s="2"/>
+      <c r="X2" s="63" t="s">
         <v>1</v>
       </c>
+      <c r="Y2" s="9"/>
       <c r="Z2" s="9"/>
-      <c r="AA2" s="9"/>
-      <c r="AB2" s="10"/>
-      <c r="AC2" s="1"/>
-    </row>
-    <row r="3" spans="2:29" ht="15.75" customHeight="1">
-      <c r="B3" s="14"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="15"/>
+      <c r="AA2" s="10"/>
+      <c r="AB2" s="1"/>
+    </row>
+    <row r="3" spans="1:28" ht="15.75" customHeight="1">
+      <c r="A3" s="67"/>
+      <c r="B3" s="68"/>
+      <c r="C3" s="68"/>
+      <c r="D3" s="57"/>
+      <c r="E3" s="1"/>
       <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
+      <c r="W3" s="1"/>
       <c r="X3" s="1"/>
       <c r="Y3" s="1"/>
       <c r="Z3" s="1"/>
       <c r="AA3" s="1"/>
       <c r="AB3" s="1"/>
-      <c r="AC3" s="1"/>
-    </row>
-    <row r="4" spans="2:29" ht="15.75" customHeight="1">
-      <c r="B4" s="14"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="15"/>
+    </row>
+    <row r="4" spans="1:28" ht="15.75" customHeight="1">
+      <c r="A4" s="67"/>
+      <c r="B4" s="68"/>
+      <c r="C4" s="68"/>
+      <c r="D4" s="57"/>
+      <c r="E4" s="1"/>
       <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
+      <c r="W4" s="1"/>
       <c r="X4" s="1"/>
       <c r="Y4" s="1"/>
       <c r="Z4" s="1"/>
       <c r="AA4" s="1"/>
       <c r="AB4" s="1"/>
-      <c r="AC4" s="1"/>
-    </row>
-    <row r="5" spans="2:29" ht="12.75">
-      <c r="B5" s="16"/>
+    </row>
+    <row r="5" spans="1:28" ht="12.75">
+      <c r="A5" s="69"/>
+      <c r="B5" s="9"/>
       <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
@@ -1068,165 +1082,165 @@
       <c r="Z5" s="1"/>
       <c r="AA5" s="1"/>
       <c r="AB5" s="1"/>
-      <c r="AC5" s="1"/>
-    </row>
-    <row r="6" spans="2:29" ht="12.75">
-      <c r="B6" s="18" t="s">
+    </row>
+    <row r="6" spans="1:28" ht="12.75">
+      <c r="A6" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="9"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="17" t="s">
+      <c r="B6" s="9"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="52" t="s">
         <v>3</v>
       </c>
+      <c r="E6" s="9"/>
       <c r="F6" s="9"/>
       <c r="G6" s="9"/>
       <c r="H6" s="9"/>
       <c r="I6" s="9"/>
       <c r="J6" s="9"/>
       <c r="K6" s="9"/>
-      <c r="L6" s="9"/>
-      <c r="M6" s="10"/>
-      <c r="N6" s="17" t="s">
+      <c r="L6" s="10"/>
+      <c r="M6" s="52" t="s">
         <v>4</v>
       </c>
+      <c r="N6" s="9"/>
       <c r="O6" s="9"/>
       <c r="P6" s="9"/>
       <c r="Q6" s="9"/>
       <c r="R6" s="9"/>
       <c r="S6" s="9"/>
-      <c r="T6" s="9"/>
-      <c r="U6" s="10"/>
-      <c r="V6" s="17" t="s">
+      <c r="T6" s="10"/>
+      <c r="U6" s="52" t="s">
         <v>5</v>
       </c>
+      <c r="V6" s="9"/>
       <c r="W6" s="9"/>
-      <c r="X6" s="9"/>
-      <c r="Y6" s="10"/>
-      <c r="Z6" s="17" t="s">
+      <c r="X6" s="10"/>
+      <c r="Y6" s="52" t="s">
         <v>6</v>
       </c>
+      <c r="Z6" s="9"/>
       <c r="AA6" s="9"/>
-      <c r="AB6" s="9"/>
-      <c r="AC6" s="10"/>
-    </row>
-    <row r="7" spans="2:29">
-      <c r="B7" s="22"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="19" t="s">
+      <c r="AB6" s="10"/>
+    </row>
+    <row r="7" spans="1:28" ht="12.75">
+      <c r="A7" s="71"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="11" t="s">
         <v>50</v>
       </c>
+      <c r="E7" s="9"/>
       <c r="F7" s="9"/>
       <c r="G7" s="9"/>
       <c r="H7" s="9"/>
       <c r="I7" s="9"/>
       <c r="J7" s="9"/>
       <c r="K7" s="9"/>
-      <c r="L7" s="9"/>
-      <c r="M7" s="10"/>
-      <c r="N7" s="20" t="s">
+      <c r="L7" s="10"/>
+      <c r="M7" s="12" t="s">
         <v>48</v>
       </c>
+      <c r="N7" s="9"/>
       <c r="O7" s="9"/>
       <c r="P7" s="9"/>
       <c r="Q7" s="9"/>
       <c r="R7" s="9"/>
       <c r="S7" s="9"/>
-      <c r="T7" s="9"/>
-      <c r="U7" s="10"/>
-      <c r="V7" s="21">
+      <c r="T7" s="10"/>
+      <c r="U7" s="70">
         <v>43739</v>
       </c>
+      <c r="V7" s="9"/>
       <c r="W7" s="9"/>
-      <c r="X7" s="9"/>
-      <c r="Y7" s="10"/>
-      <c r="Z7" s="19" t="s">
+      <c r="X7" s="10"/>
+      <c r="Y7" s="11" t="s">
         <v>7</v>
       </c>
+      <c r="Z7" s="9"/>
       <c r="AA7" s="9"/>
-      <c r="AB7" s="9"/>
-      <c r="AC7" s="10"/>
-    </row>
-    <row r="8" spans="2:29">
-      <c r="B8" s="18" t="s">
+      <c r="AB7" s="10"/>
+    </row>
+    <row r="8" spans="1:28" ht="12.75">
+      <c r="A8" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="9"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="17" t="s">
+      <c r="B8" s="9"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="52" t="s">
         <v>9</v>
       </c>
+      <c r="E8" s="9"/>
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
       <c r="H8" s="9"/>
       <c r="I8" s="9"/>
       <c r="J8" s="9"/>
       <c r="K8" s="9"/>
-      <c r="L8" s="9"/>
-      <c r="M8" s="10"/>
-      <c r="N8" s="17" t="s">
+      <c r="L8" s="10"/>
+      <c r="M8" s="52" t="s">
         <v>10</v>
       </c>
+      <c r="N8" s="9"/>
       <c r="O8" s="9"/>
       <c r="P8" s="9"/>
       <c r="Q8" s="9"/>
       <c r="R8" s="9"/>
       <c r="S8" s="9"/>
-      <c r="T8" s="9"/>
-      <c r="U8" s="10"/>
-      <c r="V8" s="17" t="s">
+      <c r="T8" s="10"/>
+      <c r="U8" s="52" t="s">
         <v>11</v>
       </c>
+      <c r="V8" s="9"/>
       <c r="W8" s="9"/>
-      <c r="X8" s="9"/>
-      <c r="Y8" s="10"/>
-      <c r="Z8" s="17" t="s">
+      <c r="X8" s="10"/>
+      <c r="Y8" s="52" t="s">
         <v>12</v>
       </c>
+      <c r="Z8" s="9"/>
       <c r="AA8" s="9"/>
-      <c r="AB8" s="9"/>
-      <c r="AC8" s="10"/>
-    </row>
-    <row r="9" spans="2:29" ht="12.75">
-      <c r="B9" s="31">
+      <c r="AB8" s="10"/>
+    </row>
+    <row r="9" spans="1:28" ht="12.75">
+      <c r="A9" s="47">
         <v>5677507</v>
       </c>
-      <c r="C9" s="9"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="19" t="s">
+      <c r="B9" s="9"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="11" t="s">
         <v>49</v>
       </c>
+      <c r="E9" s="9"/>
       <c r="F9" s="9"/>
       <c r="G9" s="9"/>
       <c r="H9" s="9"/>
       <c r="I9" s="9"/>
       <c r="J9" s="9"/>
       <c r="K9" s="9"/>
-      <c r="L9" s="9"/>
-      <c r="M9" s="10"/>
-      <c r="N9" s="47" t="s">
+      <c r="L9" s="10"/>
+      <c r="M9" s="53" t="s">
         <v>47</v>
       </c>
+      <c r="N9" s="9"/>
       <c r="O9" s="9"/>
       <c r="P9" s="9"/>
       <c r="Q9" s="9"/>
       <c r="R9" s="9"/>
       <c r="S9" s="9"/>
-      <c r="T9" s="9"/>
-      <c r="U9" s="10"/>
-      <c r="V9" s="20"/>
+      <c r="T9" s="10"/>
+      <c r="U9" s="12"/>
+      <c r="V9" s="9"/>
       <c r="W9" s="9"/>
-      <c r="X9" s="9"/>
-      <c r="Y9" s="10"/>
-      <c r="Z9" s="19" t="s">
+      <c r="X9" s="10"/>
+      <c r="Y9" s="11" t="s">
         <v>13</v>
       </c>
+      <c r="Z9" s="9"/>
       <c r="AA9" s="9"/>
-      <c r="AB9" s="9"/>
-      <c r="AC9" s="10"/>
-    </row>
-    <row r="10" spans="2:29">
+      <c r="AB9" s="10"/>
+    </row>
+    <row r="10" spans="1:28" ht="12.75">
+      <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
@@ -1254,708 +1268,708 @@
       <c r="Z10" s="3"/>
       <c r="AA10" s="3"/>
       <c r="AB10" s="3"/>
-      <c r="AC10" s="3"/>
-    </row>
-    <row r="11" spans="2:29" ht="15.75" customHeight="1">
-      <c r="B11" s="32" t="s">
+    </row>
+    <row r="11" spans="1:28" ht="15.75" customHeight="1">
+      <c r="A11" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="10"/>
-      <c r="D11" s="27" t="s">
+      <c r="B11" s="10"/>
+      <c r="C11" s="61" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="9"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="27" t="s">
+      <c r="D11" s="9"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="61" t="s">
         <v>16</v>
       </c>
+      <c r="G11" s="9"/>
       <c r="H11" s="9"/>
       <c r="I11" s="9"/>
       <c r="J11" s="9"/>
       <c r="K11" s="9"/>
       <c r="L11" s="9"/>
       <c r="M11" s="9"/>
-      <c r="N11" s="9"/>
-      <c r="O11" s="10"/>
-      <c r="P11" s="29" t="s">
+      <c r="N11" s="10"/>
+      <c r="O11" s="54" t="s">
         <v>17</v>
       </c>
-      <c r="Q11" s="9"/>
-      <c r="R11" s="10"/>
-      <c r="S11" s="29" t="s">
+      <c r="P11" s="9"/>
+      <c r="Q11" s="10"/>
+      <c r="R11" s="54" t="s">
         <v>18</v>
       </c>
-      <c r="T11" s="9"/>
-      <c r="U11" s="10"/>
-      <c r="V11" s="49" t="s">
+      <c r="S11" s="9"/>
+      <c r="T11" s="10"/>
+      <c r="U11" s="55" t="s">
         <v>19</v>
       </c>
-      <c r="W11" s="48"/>
-      <c r="X11" s="48"/>
-      <c r="Y11" s="15"/>
-      <c r="Z11" s="29" t="s">
+      <c r="V11" s="56"/>
+      <c r="W11" s="56"/>
+      <c r="X11" s="57"/>
+      <c r="Y11" s="54" t="s">
         <v>20</v>
       </c>
+      <c r="Z11" s="9"/>
       <c r="AA11" s="9"/>
-      <c r="AB11" s="9"/>
-      <c r="AC11" s="10"/>
-    </row>
-    <row r="12" spans="2:29" ht="15.75" customHeight="1">
-      <c r="B12" s="28">
+      <c r="AB11" s="10"/>
+    </row>
+    <row r="12" spans="1:28" ht="15.75" customHeight="1">
+      <c r="A12" s="45">
         <v>1</v>
       </c>
-      <c r="C12" s="10"/>
-      <c r="D12" s="26" t="s">
+      <c r="B12" s="10"/>
+      <c r="C12" s="49" t="s">
         <v>21</v>
       </c>
-      <c r="E12" s="9"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="30" t="s">
+      <c r="D12" s="9"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="51" t="s">
         <v>22</v>
       </c>
+      <c r="G12" s="9"/>
       <c r="H12" s="9"/>
       <c r="I12" s="9"/>
       <c r="J12" s="9"/>
       <c r="K12" s="9"/>
       <c r="L12" s="9"/>
       <c r="M12" s="9"/>
-      <c r="N12" s="9"/>
-      <c r="O12" s="10"/>
-      <c r="P12" s="19">
+      <c r="N12" s="10"/>
+      <c r="O12" s="11">
         <v>4</v>
       </c>
-      <c r="Q12" s="9"/>
-      <c r="R12" s="10"/>
-      <c r="S12" s="20"/>
-      <c r="T12" s="9"/>
-      <c r="U12" s="10"/>
-      <c r="V12" s="56">
+      <c r="P12" s="9"/>
+      <c r="Q12" s="10"/>
+      <c r="R12" s="12"/>
+      <c r="S12" s="9"/>
+      <c r="T12" s="10"/>
+      <c r="U12" s="25">
         <v>514183</v>
       </c>
-      <c r="W12" s="57"/>
-      <c r="X12" s="57"/>
-      <c r="Y12" s="58"/>
-      <c r="Z12" s="63"/>
-      <c r="AA12" s="64"/>
-      <c r="AB12" s="64"/>
-      <c r="AC12" s="65"/>
-    </row>
-    <row r="13" spans="2:29" ht="15.75" customHeight="1">
-      <c r="B13" s="28">
+      <c r="V12" s="26"/>
+      <c r="W12" s="26"/>
+      <c r="X12" s="27"/>
+      <c r="Y12" s="38"/>
+      <c r="Z12" s="39"/>
+      <c r="AA12" s="39"/>
+      <c r="AB12" s="40"/>
+    </row>
+    <row r="13" spans="1:28" ht="15.75" customHeight="1">
+      <c r="A13" s="45">
         <v>2</v>
       </c>
-      <c r="C13" s="10"/>
-      <c r="D13" s="23" t="s">
+      <c r="B13" s="10"/>
+      <c r="C13" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="E13" s="9"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="23" t="s">
+      <c r="D13" s="9"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="58" t="s">
         <v>24</v>
       </c>
+      <c r="G13" s="9"/>
       <c r="H13" s="9"/>
       <c r="I13" s="9"/>
       <c r="J13" s="9"/>
       <c r="K13" s="9"/>
       <c r="L13" s="9"/>
       <c r="M13" s="9"/>
-      <c r="N13" s="9"/>
-      <c r="O13" s="10"/>
-      <c r="P13" s="19">
+      <c r="N13" s="10"/>
+      <c r="O13" s="11">
         <v>4</v>
       </c>
-      <c r="Q13" s="9"/>
-      <c r="R13" s="10"/>
-      <c r="S13" s="20"/>
-      <c r="T13" s="9"/>
-      <c r="U13" s="10"/>
-      <c r="V13" s="50">
+      <c r="P13" s="9"/>
+      <c r="Q13" s="10"/>
+      <c r="R13" s="12"/>
+      <c r="S13" s="9"/>
+      <c r="T13" s="10"/>
+      <c r="U13" s="28">
         <v>1199999</v>
       </c>
-      <c r="W13" s="51"/>
-      <c r="X13" s="51"/>
-      <c r="Y13" s="54"/>
-      <c r="Z13" s="69"/>
-      <c r="AA13" s="70"/>
-      <c r="AB13" s="70"/>
-      <c r="AC13" s="71"/>
-    </row>
-    <row r="14" spans="2:29" ht="15.75" customHeight="1">
-      <c r="B14" s="28">
+      <c r="V13" s="29"/>
+      <c r="W13" s="29"/>
+      <c r="X13" s="30"/>
+      <c r="Y13" s="35"/>
+      <c r="Z13" s="36"/>
+      <c r="AA13" s="36"/>
+      <c r="AB13" s="37"/>
+    </row>
+    <row r="14" spans="1:28" ht="15.75" customHeight="1">
+      <c r="A14" s="45">
         <v>3</v>
       </c>
-      <c r="C14" s="10"/>
-      <c r="D14" s="26" t="s">
+      <c r="B14" s="10"/>
+      <c r="C14" s="49" t="s">
         <v>25</v>
       </c>
-      <c r="E14" s="9"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="23" t="s">
+      <c r="D14" s="9"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="58" t="s">
         <v>44</v>
       </c>
+      <c r="G14" s="9"/>
       <c r="H14" s="9"/>
       <c r="I14" s="9"/>
       <c r="J14" s="9"/>
       <c r="K14" s="9"/>
       <c r="L14" s="9"/>
       <c r="M14" s="9"/>
-      <c r="N14" s="9"/>
-      <c r="O14" s="10"/>
-      <c r="P14" s="19">
+      <c r="N14" s="10"/>
+      <c r="O14" s="11">
         <v>1</v>
       </c>
-      <c r="Q14" s="9"/>
-      <c r="R14" s="10"/>
-      <c r="S14" s="20"/>
-      <c r="T14" s="9"/>
-      <c r="U14" s="10"/>
-      <c r="V14" s="50">
+      <c r="P14" s="9"/>
+      <c r="Q14" s="10"/>
+      <c r="R14" s="12"/>
+      <c r="S14" s="9"/>
+      <c r="T14" s="10"/>
+      <c r="U14" s="28">
         <v>21000</v>
       </c>
-      <c r="W14" s="51"/>
-      <c r="X14" s="51"/>
-      <c r="Y14" s="54"/>
-      <c r="Z14" s="66"/>
-      <c r="AA14" s="67"/>
-      <c r="AB14" s="67"/>
-      <c r="AC14" s="68"/>
-    </row>
-    <row r="15" spans="2:29" ht="15.75" customHeight="1">
-      <c r="B15" s="28">
+      <c r="V14" s="29"/>
+      <c r="W14" s="29"/>
+      <c r="X14" s="30"/>
+      <c r="Y14" s="41"/>
+      <c r="Z14" s="42"/>
+      <c r="AA14" s="42"/>
+      <c r="AB14" s="43"/>
+    </row>
+    <row r="15" spans="1:28" ht="15.75" customHeight="1">
+      <c r="A15" s="45">
         <v>4</v>
       </c>
-      <c r="C15" s="10"/>
-      <c r="D15" s="24" t="s">
+      <c r="B15" s="10"/>
+      <c r="C15" s="59" t="s">
         <v>26</v>
       </c>
-      <c r="E15" s="9"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="23" t="s">
+      <c r="D15" s="9"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="58" t="s">
         <v>27</v>
       </c>
+      <c r="G15" s="9"/>
       <c r="H15" s="9"/>
       <c r="I15" s="9"/>
       <c r="J15" s="9"/>
       <c r="K15" s="9"/>
       <c r="L15" s="9"/>
       <c r="M15" s="9"/>
-      <c r="N15" s="9"/>
-      <c r="O15" s="10"/>
-      <c r="P15" s="19">
+      <c r="N15" s="10"/>
+      <c r="O15" s="11">
         <v>1</v>
       </c>
-      <c r="Q15" s="9"/>
-      <c r="R15" s="10"/>
-      <c r="S15" s="20"/>
-      <c r="T15" s="9"/>
-      <c r="U15" s="10"/>
-      <c r="V15" s="50">
+      <c r="P15" s="9"/>
+      <c r="Q15" s="10"/>
+      <c r="R15" s="12"/>
+      <c r="S15" s="9"/>
+      <c r="T15" s="10"/>
+      <c r="U15" s="28">
         <v>59200</v>
       </c>
-      <c r="W15" s="51"/>
-      <c r="X15" s="51"/>
-      <c r="Y15" s="54"/>
-      <c r="Z15" s="69"/>
-      <c r="AA15" s="70"/>
-      <c r="AB15" s="70"/>
-      <c r="AC15" s="71"/>
-    </row>
-    <row r="16" spans="2:29" ht="15.75" customHeight="1">
-      <c r="B16" s="28">
+      <c r="V15" s="29"/>
+      <c r="W15" s="29"/>
+      <c r="X15" s="30"/>
+      <c r="Y15" s="35"/>
+      <c r="Z15" s="36"/>
+      <c r="AA15" s="36"/>
+      <c r="AB15" s="37"/>
+    </row>
+    <row r="16" spans="1:28" ht="15.75" customHeight="1">
+      <c r="A16" s="45">
         <v>5</v>
       </c>
-      <c r="C16" s="10"/>
-      <c r="D16" s="26" t="s">
+      <c r="B16" s="10"/>
+      <c r="C16" s="49" t="s">
         <v>28</v>
       </c>
-      <c r="E16" s="9"/>
-      <c r="F16" s="10"/>
-      <c r="G16" s="23" t="s">
+      <c r="D16" s="9"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="58" t="s">
         <v>29</v>
       </c>
+      <c r="G16" s="9"/>
       <c r="H16" s="9"/>
       <c r="I16" s="9"/>
       <c r="J16" s="9"/>
       <c r="K16" s="9"/>
       <c r="L16" s="9"/>
       <c r="M16" s="9"/>
-      <c r="N16" s="9"/>
-      <c r="O16" s="10"/>
-      <c r="P16" s="19">
+      <c r="N16" s="10"/>
+      <c r="O16" s="11">
         <v>1</v>
       </c>
-      <c r="Q16" s="9"/>
-      <c r="R16" s="10"/>
-      <c r="S16" s="20"/>
-      <c r="T16" s="9"/>
-      <c r="U16" s="10"/>
-      <c r="V16" s="50">
+      <c r="P16" s="9"/>
+      <c r="Q16" s="10"/>
+      <c r="R16" s="12"/>
+      <c r="S16" s="9"/>
+      <c r="T16" s="10"/>
+      <c r="U16" s="28">
         <v>385000</v>
       </c>
-      <c r="W16" s="51"/>
-      <c r="X16" s="51"/>
-      <c r="Y16" s="54"/>
-      <c r="Z16" s="69"/>
-      <c r="AA16" s="70"/>
-      <c r="AB16" s="70"/>
-      <c r="AC16" s="71"/>
-    </row>
-    <row r="17" spans="2:29" ht="15.75" customHeight="1">
-      <c r="B17" s="28">
+      <c r="V16" s="29"/>
+      <c r="W16" s="29"/>
+      <c r="X16" s="30"/>
+      <c r="Y16" s="35"/>
+      <c r="Z16" s="36"/>
+      <c r="AA16" s="36"/>
+      <c r="AB16" s="37"/>
+    </row>
+    <row r="17" spans="1:28" ht="15.75" customHeight="1">
+      <c r="A17" s="45">
         <v>6</v>
       </c>
-      <c r="C17" s="10"/>
-      <c r="D17" s="26" t="s">
+      <c r="B17" s="10"/>
+      <c r="C17" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="E17" s="9"/>
-      <c r="F17" s="10"/>
-      <c r="G17" s="25" t="s">
+      <c r="D17" s="9"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="60" t="s">
         <v>31</v>
       </c>
+      <c r="G17" s="9"/>
       <c r="H17" s="9"/>
       <c r="I17" s="9"/>
       <c r="J17" s="9"/>
       <c r="K17" s="9"/>
       <c r="L17" s="9"/>
       <c r="M17" s="9"/>
-      <c r="N17" s="9"/>
-      <c r="O17" s="10"/>
-      <c r="P17" s="19">
+      <c r="N17" s="10"/>
+      <c r="O17" s="11">
         <v>4</v>
       </c>
-      <c r="Q17" s="9"/>
-      <c r="R17" s="10"/>
-      <c r="S17" s="20"/>
-      <c r="T17" s="9"/>
-      <c r="U17" s="10"/>
-      <c r="V17" s="50" t="s">
+      <c r="P17" s="9"/>
+      <c r="Q17" s="10"/>
+      <c r="R17" s="12"/>
+      <c r="S17" s="9"/>
+      <c r="T17" s="10"/>
+      <c r="U17" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="W17" s="51"/>
-      <c r="X17" s="51"/>
-      <c r="Y17" s="54"/>
-      <c r="Z17" s="69"/>
-      <c r="AA17" s="70"/>
-      <c r="AB17" s="70"/>
-      <c r="AC17" s="71"/>
-    </row>
-    <row r="18" spans="2:29" ht="15.75" customHeight="1">
-      <c r="B18" s="28">
+      <c r="V17" s="29"/>
+      <c r="W17" s="29"/>
+      <c r="X17" s="30"/>
+      <c r="Y17" s="35"/>
+      <c r="Z17" s="36"/>
+      <c r="AA17" s="36"/>
+      <c r="AB17" s="37"/>
+    </row>
+    <row r="18" spans="1:28" ht="15.75" customHeight="1">
+      <c r="A18" s="45">
         <v>7</v>
       </c>
-      <c r="C18" s="10"/>
-      <c r="D18" s="26" t="s">
+      <c r="B18" s="10"/>
+      <c r="C18" s="49" t="s">
         <v>32</v>
       </c>
-      <c r="E18" s="9"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="26" t="s">
+      <c r="D18" s="9"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="49" t="s">
         <v>33</v>
       </c>
+      <c r="G18" s="9"/>
       <c r="H18" s="9"/>
       <c r="I18" s="9"/>
       <c r="J18" s="9"/>
       <c r="K18" s="9"/>
       <c r="L18" s="9"/>
       <c r="M18" s="9"/>
-      <c r="N18" s="9"/>
-      <c r="O18" s="10"/>
-      <c r="P18" s="19">
+      <c r="N18" s="10"/>
+      <c r="O18" s="11">
         <v>4</v>
       </c>
-      <c r="Q18" s="9"/>
-      <c r="R18" s="10"/>
-      <c r="S18" s="20"/>
-      <c r="T18" s="9"/>
-      <c r="U18" s="10"/>
-      <c r="V18" s="50">
+      <c r="P18" s="9"/>
+      <c r="Q18" s="10"/>
+      <c r="R18" s="12"/>
+      <c r="S18" s="9"/>
+      <c r="T18" s="10"/>
+      <c r="U18" s="28">
         <v>2099099</v>
       </c>
-      <c r="W18" s="51"/>
-      <c r="X18" s="51"/>
-      <c r="Y18" s="54"/>
-      <c r="Z18" s="69"/>
-      <c r="AA18" s="70"/>
-      <c r="AB18" s="70"/>
-      <c r="AC18" s="71"/>
-    </row>
-    <row r="19" spans="2:29" ht="15.75" customHeight="1">
-      <c r="B19" s="28">
+      <c r="V18" s="29"/>
+      <c r="W18" s="29"/>
+      <c r="X18" s="30"/>
+      <c r="Y18" s="35"/>
+      <c r="Z18" s="36"/>
+      <c r="AA18" s="36"/>
+      <c r="AB18" s="37"/>
+    </row>
+    <row r="19" spans="1:28" ht="15.75" customHeight="1">
+      <c r="A19" s="45">
         <v>8</v>
       </c>
-      <c r="C19" s="10"/>
-      <c r="D19" s="26" t="s">
+      <c r="B19" s="10"/>
+      <c r="C19" s="49" t="s">
         <v>34</v>
       </c>
-      <c r="E19" s="9"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="26" t="s">
+      <c r="D19" s="9"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="49" t="s">
         <v>35</v>
       </c>
+      <c r="G19" s="9"/>
       <c r="H19" s="9"/>
       <c r="I19" s="9"/>
       <c r="J19" s="9"/>
       <c r="K19" s="9"/>
       <c r="L19" s="9"/>
       <c r="M19" s="9"/>
-      <c r="N19" s="9"/>
-      <c r="O19" s="10"/>
-      <c r="P19" s="19">
+      <c r="N19" s="10"/>
+      <c r="O19" s="11">
         <v>4</v>
       </c>
-      <c r="Q19" s="9"/>
-      <c r="R19" s="10"/>
-      <c r="S19" s="20"/>
-      <c r="T19" s="9"/>
-      <c r="U19" s="10"/>
-      <c r="V19" s="50" t="s">
+      <c r="P19" s="9"/>
+      <c r="Q19" s="10"/>
+      <c r="R19" s="12"/>
+      <c r="S19" s="9"/>
+      <c r="T19" s="10"/>
+      <c r="U19" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="W19" s="51"/>
-      <c r="X19" s="51"/>
-      <c r="Y19" s="54"/>
-      <c r="Z19" s="69"/>
-      <c r="AA19" s="70"/>
-      <c r="AB19" s="70"/>
-      <c r="AC19" s="71"/>
-    </row>
-    <row r="20" spans="2:29" ht="15">
-      <c r="B20" s="28">
+      <c r="V19" s="29"/>
+      <c r="W19" s="29"/>
+      <c r="X19" s="30"/>
+      <c r="Y19" s="35"/>
+      <c r="Z19" s="36"/>
+      <c r="AA19" s="36"/>
+      <c r="AB19" s="37"/>
+    </row>
+    <row r="20" spans="1:28" ht="15">
+      <c r="A20" s="45">
         <v>22</v>
       </c>
-      <c r="C20" s="10"/>
-      <c r="D20" s="33" t="s">
+      <c r="B20" s="10"/>
+      <c r="C20" s="50" t="s">
         <v>36</v>
       </c>
-      <c r="E20" s="9"/>
-      <c r="F20" s="10"/>
-      <c r="G20" s="33" t="s">
+      <c r="D20" s="9"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="50" t="s">
         <v>37</v>
       </c>
+      <c r="G20" s="9"/>
       <c r="H20" s="9"/>
       <c r="I20" s="9"/>
       <c r="J20" s="9"/>
       <c r="K20" s="9"/>
       <c r="L20" s="9"/>
       <c r="M20" s="9"/>
-      <c r="N20" s="9"/>
-      <c r="O20" s="10"/>
-      <c r="P20" s="20">
+      <c r="N20" s="10"/>
+      <c r="O20" s="12">
         <v>4</v>
       </c>
-      <c r="Q20" s="9"/>
-      <c r="R20" s="10"/>
-      <c r="S20" s="20"/>
-      <c r="T20" s="9"/>
-      <c r="U20" s="10"/>
-      <c r="V20" s="52">
+      <c r="P20" s="9"/>
+      <c r="Q20" s="10"/>
+      <c r="R20" s="12"/>
+      <c r="S20" s="9"/>
+      <c r="T20" s="10"/>
+      <c r="U20" s="31">
         <v>147612</v>
       </c>
-      <c r="W20" s="53"/>
-      <c r="X20" s="53"/>
-      <c r="Y20" s="55"/>
-      <c r="Z20" s="69"/>
-      <c r="AA20" s="70"/>
-      <c r="AB20" s="70"/>
-      <c r="AC20" s="71"/>
-    </row>
-    <row r="21" spans="2:29" ht="15">
-      <c r="B21" s="28">
+      <c r="V20" s="32"/>
+      <c r="W20" s="32"/>
+      <c r="X20" s="33"/>
+      <c r="Y20" s="35"/>
+      <c r="Z20" s="36"/>
+      <c r="AA20" s="36"/>
+      <c r="AB20" s="37"/>
+    </row>
+    <row r="21" spans="1:28" ht="15">
+      <c r="A21" s="45">
         <v>22</v>
       </c>
-      <c r="C21" s="10"/>
-      <c r="D21" s="33" t="s">
+      <c r="B21" s="10"/>
+      <c r="C21" s="50" t="s">
         <v>46</v>
       </c>
-      <c r="E21" s="9"/>
-      <c r="F21" s="10"/>
-      <c r="G21" s="33" t="s">
+      <c r="D21" s="9"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="50" t="s">
         <v>38</v>
       </c>
+      <c r="G21" s="9"/>
       <c r="H21" s="9"/>
       <c r="I21" s="9"/>
       <c r="J21" s="9"/>
       <c r="K21" s="9"/>
       <c r="L21" s="9"/>
       <c r="M21" s="9"/>
-      <c r="N21" s="9"/>
-      <c r="O21" s="10"/>
-      <c r="P21" s="20">
+      <c r="N21" s="10"/>
+      <c r="O21" s="12">
         <v>4</v>
       </c>
-      <c r="Q21" s="9"/>
-      <c r="R21" s="10"/>
-      <c r="S21" s="46"/>
+      <c r="P21" s="9"/>
+      <c r="Q21" s="10"/>
+      <c r="R21" s="44"/>
+      <c r="S21" s="6"/>
       <c r="T21" s="6"/>
-      <c r="U21" s="6"/>
-      <c r="V21" s="59" t="s">
+      <c r="U21" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="W21" s="60"/>
-      <c r="X21" s="60"/>
-      <c r="Y21" s="61"/>
-      <c r="Z21" s="69"/>
-      <c r="AA21" s="70"/>
-      <c r="AB21" s="70"/>
-      <c r="AC21" s="71"/>
-    </row>
-    <row r="22" spans="2:29" ht="12.75">
-      <c r="B22" s="38"/>
-      <c r="C22" s="39"/>
-      <c r="D22" s="39"/>
-      <c r="E22" s="39"/>
-      <c r="F22" s="39"/>
-      <c r="G22" s="39"/>
-      <c r="H22" s="39"/>
-      <c r="I22" s="39"/>
-      <c r="J22" s="39"/>
-      <c r="K22" s="39"/>
-      <c r="L22" s="39"/>
-      <c r="M22" s="39"/>
-      <c r="N22" s="39"/>
-      <c r="O22" s="39"/>
-      <c r="P22" s="39"/>
-      <c r="Q22" s="39"/>
-      <c r="R22" s="39"/>
-      <c r="S22" s="39"/>
-      <c r="T22" s="39"/>
-      <c r="U22" s="40"/>
-      <c r="V22" s="35" t="s">
+      <c r="V21" s="23"/>
+      <c r="W21" s="23"/>
+      <c r="X21" s="24"/>
+      <c r="Y21" s="35"/>
+      <c r="Z21" s="36"/>
+      <c r="AA21" s="36"/>
+      <c r="AB21" s="37"/>
+    </row>
+    <row r="22" spans="1:28" ht="12.75">
+      <c r="A22" s="13"/>
+      <c r="B22" s="14"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="14"/>
+      <c r="I22" s="14"/>
+      <c r="J22" s="14"/>
+      <c r="K22" s="14"/>
+      <c r="L22" s="14"/>
+      <c r="M22" s="14"/>
+      <c r="N22" s="14"/>
+      <c r="O22" s="14"/>
+      <c r="P22" s="14"/>
+      <c r="Q22" s="14"/>
+      <c r="R22" s="14"/>
+      <c r="S22" s="14"/>
+      <c r="T22" s="15"/>
+      <c r="U22" s="8" t="s">
         <v>39</v>
       </c>
+      <c r="V22" s="9"/>
       <c r="W22" s="9"/>
-      <c r="X22" s="9"/>
-      <c r="Y22" s="10"/>
-      <c r="Z22" s="34">
-        <f>SUM(V12,V13,V14,V15,V16,V18,V20)</f>
+      <c r="X22" s="10"/>
+      <c r="Y22" s="34">
+        <f>SUM(U12,U13,U14,U15,U16,U18,U20)</f>
         <v>4426093</v>
       </c>
+      <c r="Z22" s="9"/>
       <c r="AA22" s="9"/>
-      <c r="AB22" s="9"/>
-      <c r="AC22" s="10"/>
-    </row>
-    <row r="23" spans="2:29" ht="12.75">
-      <c r="B23" s="37"/>
-      <c r="C23" s="41"/>
-      <c r="D23" s="41"/>
-      <c r="E23" s="41"/>
-      <c r="F23" s="41"/>
-      <c r="G23" s="41"/>
-      <c r="H23" s="41"/>
-      <c r="I23" s="41"/>
-      <c r="J23" s="41"/>
-      <c r="K23" s="41"/>
-      <c r="L23" s="41"/>
-      <c r="M23" s="41"/>
-      <c r="N23" s="41"/>
-      <c r="O23" s="41"/>
-      <c r="P23" s="41"/>
-      <c r="Q23" s="41"/>
-      <c r="R23" s="41"/>
-      <c r="S23" s="41"/>
-      <c r="T23" s="41"/>
-      <c r="U23" s="42"/>
-      <c r="V23" s="35" t="s">
+      <c r="AB22" s="10"/>
+    </row>
+    <row r="23" spans="1:28" ht="12.75">
+      <c r="A23" s="16"/>
+      <c r="B23" s="17"/>
+      <c r="C23" s="17"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="17"/>
+      <c r="G23" s="17"/>
+      <c r="H23" s="17"/>
+      <c r="I23" s="17"/>
+      <c r="J23" s="17"/>
+      <c r="K23" s="17"/>
+      <c r="L23" s="17"/>
+      <c r="M23" s="17"/>
+      <c r="N23" s="17"/>
+      <c r="O23" s="17"/>
+      <c r="P23" s="17"/>
+      <c r="Q23" s="17"/>
+      <c r="R23" s="17"/>
+      <c r="S23" s="17"/>
+      <c r="T23" s="18"/>
+      <c r="U23" s="8" t="s">
         <v>40</v>
       </c>
+      <c r="V23" s="9"/>
       <c r="W23" s="9"/>
-      <c r="X23" s="9"/>
-      <c r="Y23" s="10"/>
-      <c r="Z23" s="34"/>
+      <c r="X23" s="10"/>
+      <c r="Y23" s="34"/>
+      <c r="Z23" s="9"/>
       <c r="AA23" s="9"/>
-      <c r="AB23" s="9"/>
-      <c r="AC23" s="10"/>
-    </row>
-    <row r="24" spans="2:29" ht="12.75">
-      <c r="B24" s="37"/>
-      <c r="C24" s="41"/>
-      <c r="D24" s="41"/>
-      <c r="E24" s="41"/>
-      <c r="F24" s="41"/>
-      <c r="G24" s="41"/>
-      <c r="H24" s="41"/>
-      <c r="I24" s="41"/>
-      <c r="J24" s="41"/>
-      <c r="K24" s="41"/>
-      <c r="L24" s="41"/>
-      <c r="M24" s="41"/>
-      <c r="N24" s="41"/>
-      <c r="O24" s="41"/>
-      <c r="P24" s="41"/>
-      <c r="Q24" s="41"/>
-      <c r="R24" s="41"/>
-      <c r="S24" s="41"/>
-      <c r="T24" s="41"/>
-      <c r="U24" s="42"/>
-      <c r="V24" s="35" t="s">
+      <c r="AB23" s="10"/>
+    </row>
+    <row r="24" spans="1:28" ht="12.75">
+      <c r="A24" s="16"/>
+      <c r="B24" s="17"/>
+      <c r="C24" s="17"/>
+      <c r="D24" s="17"/>
+      <c r="E24" s="17"/>
+      <c r="F24" s="17"/>
+      <c r="G24" s="17"/>
+      <c r="H24" s="17"/>
+      <c r="I24" s="17"/>
+      <c r="J24" s="17"/>
+      <c r="K24" s="17"/>
+      <c r="L24" s="17"/>
+      <c r="M24" s="17"/>
+      <c r="N24" s="17"/>
+      <c r="O24" s="17"/>
+      <c r="P24" s="17"/>
+      <c r="Q24" s="17"/>
+      <c r="R24" s="17"/>
+      <c r="S24" s="17"/>
+      <c r="T24" s="18"/>
+      <c r="U24" s="8" t="s">
         <v>41</v>
       </c>
+      <c r="V24" s="9"/>
       <c r="W24" s="9"/>
-      <c r="X24" s="9"/>
-      <c r="Y24" s="10"/>
-      <c r="Z24" s="34"/>
+      <c r="X24" s="10"/>
+      <c r="Y24" s="34"/>
+      <c r="Z24" s="9"/>
       <c r="AA24" s="9"/>
-      <c r="AB24" s="9"/>
-      <c r="AC24" s="10"/>
-    </row>
-    <row r="25" spans="2:29" ht="12.75">
-      <c r="B25" s="43"/>
-      <c r="C25" s="44"/>
-      <c r="D25" s="44"/>
-      <c r="E25" s="44"/>
-      <c r="F25" s="44"/>
-      <c r="G25" s="44"/>
-      <c r="H25" s="44"/>
-      <c r="I25" s="44"/>
-      <c r="J25" s="44"/>
-      <c r="K25" s="44"/>
-      <c r="L25" s="44"/>
-      <c r="M25" s="44"/>
-      <c r="N25" s="44"/>
-      <c r="O25" s="44"/>
-      <c r="P25" s="44"/>
-      <c r="Q25" s="44"/>
-      <c r="R25" s="44"/>
-      <c r="S25" s="44"/>
-      <c r="T25" s="44"/>
-      <c r="U25" s="45"/>
-      <c r="V25" s="35" t="s">
+      <c r="AB24" s="10"/>
+    </row>
+    <row r="25" spans="1:28" ht="12.75">
+      <c r="A25" s="19"/>
+      <c r="B25" s="20"/>
+      <c r="C25" s="20"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="20"/>
+      <c r="H25" s="20"/>
+      <c r="I25" s="20"/>
+      <c r="J25" s="20"/>
+      <c r="K25" s="20"/>
+      <c r="L25" s="20"/>
+      <c r="M25" s="20"/>
+      <c r="N25" s="20"/>
+      <c r="O25" s="20"/>
+      <c r="P25" s="20"/>
+      <c r="Q25" s="20"/>
+      <c r="R25" s="20"/>
+      <c r="S25" s="20"/>
+      <c r="T25" s="21"/>
+      <c r="U25" s="8" t="s">
         <v>42</v>
       </c>
+      <c r="V25" s="9"/>
       <c r="W25" s="9"/>
-      <c r="X25" s="9"/>
-      <c r="Y25" s="10"/>
-      <c r="Z25" s="34"/>
+      <c r="X25" s="10"/>
+      <c r="Y25" s="34"/>
+      <c r="Z25" s="9"/>
       <c r="AA25" s="9"/>
-      <c r="AB25" s="9"/>
-      <c r="AC25" s="10"/>
-    </row>
-    <row r="26" spans="2:29" ht="12.75">
-      <c r="V26" s="62" t="s">
+      <c r="AB25" s="10"/>
+    </row>
+    <row r="26" spans="1:28" ht="12.75">
+      <c r="U26" s="5" t="s">
         <v>43</v>
       </c>
+      <c r="V26" s="6"/>
       <c r="W26" s="6"/>
-      <c r="X26" s="6"/>
-      <c r="Y26" s="7"/>
+      <c r="X26" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="110">
-    <mergeCell ref="V26:Y26"/>
-    <mergeCell ref="V22:Y22"/>
-    <mergeCell ref="P19:R19"/>
-    <mergeCell ref="P20:R20"/>
-    <mergeCell ref="P21:R21"/>
-    <mergeCell ref="B22:U25"/>
-    <mergeCell ref="V21:Y21"/>
-    <mergeCell ref="V12:Y12"/>
-    <mergeCell ref="V13:Y13"/>
-    <mergeCell ref="V14:Y14"/>
-    <mergeCell ref="V15:Y15"/>
-    <mergeCell ref="V16:Y16"/>
-    <mergeCell ref="V17:Y17"/>
-    <mergeCell ref="V18:Y18"/>
-    <mergeCell ref="V19:Y19"/>
-    <mergeCell ref="V20:Y20"/>
-    <mergeCell ref="Z25:AC25"/>
-    <mergeCell ref="Z24:AC24"/>
-    <mergeCell ref="Z23:AC23"/>
-    <mergeCell ref="Z22:AC22"/>
-    <mergeCell ref="Z21:AC21"/>
-    <mergeCell ref="V23:Y23"/>
-    <mergeCell ref="V24:Y24"/>
-    <mergeCell ref="V25:Y25"/>
-    <mergeCell ref="Z12:AC12"/>
-    <mergeCell ref="Z13:AC13"/>
-    <mergeCell ref="Z14:AC14"/>
-    <mergeCell ref="Z15:AC15"/>
-    <mergeCell ref="Z16:AC16"/>
-    <mergeCell ref="Z17:AC17"/>
-    <mergeCell ref="Z18:AC18"/>
-    <mergeCell ref="Z19:AC19"/>
-    <mergeCell ref="S20:U20"/>
-    <mergeCell ref="S21:U21"/>
-    <mergeCell ref="P15:R15"/>
-    <mergeCell ref="S14:U14"/>
-    <mergeCell ref="S15:U15"/>
-    <mergeCell ref="P17:R17"/>
-    <mergeCell ref="P18:R18"/>
-    <mergeCell ref="S19:U19"/>
-    <mergeCell ref="S13:U13"/>
-    <mergeCell ref="S12:U12"/>
-    <mergeCell ref="P14:R14"/>
-    <mergeCell ref="Z20:AC20"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="D19:F19"/>
-    <mergeCell ref="G19:O19"/>
-    <mergeCell ref="G20:O20"/>
-    <mergeCell ref="D20:F20"/>
-    <mergeCell ref="D21:F21"/>
-    <mergeCell ref="G21:O21"/>
-    <mergeCell ref="D12:F12"/>
-    <mergeCell ref="G12:O12"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="P12:R12"/>
-    <mergeCell ref="P13:R13"/>
-    <mergeCell ref="N8:U8"/>
-    <mergeCell ref="N9:U9"/>
-    <mergeCell ref="Z8:AC8"/>
-    <mergeCell ref="Z9:AC9"/>
-    <mergeCell ref="Z11:AC11"/>
-    <mergeCell ref="V8:Y8"/>
-    <mergeCell ref="V9:Y9"/>
-    <mergeCell ref="S11:U11"/>
-    <mergeCell ref="V11:Y11"/>
-    <mergeCell ref="P11:R11"/>
-    <mergeCell ref="P16:R16"/>
-    <mergeCell ref="G16:O16"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:F16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D18:F18"/>
-    <mergeCell ref="S17:U17"/>
-    <mergeCell ref="S16:U16"/>
-    <mergeCell ref="S18:U18"/>
-    <mergeCell ref="G13:O13"/>
-    <mergeCell ref="G14:O14"/>
-    <mergeCell ref="G15:O15"/>
-    <mergeCell ref="D15:F15"/>
-    <mergeCell ref="G17:O17"/>
-    <mergeCell ref="D17:F17"/>
-    <mergeCell ref="G18:O18"/>
-    <mergeCell ref="E8:M8"/>
-    <mergeCell ref="E9:M9"/>
-    <mergeCell ref="D13:F13"/>
-    <mergeCell ref="D11:F11"/>
-    <mergeCell ref="G11:O11"/>
-    <mergeCell ref="D14:F14"/>
-    <mergeCell ref="Y1:AB1"/>
-    <mergeCell ref="Y2:AB2"/>
-    <mergeCell ref="B1:E5"/>
-    <mergeCell ref="N6:U6"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="E6:M6"/>
-    <mergeCell ref="Z7:AC7"/>
-    <mergeCell ref="V6:Y6"/>
-    <mergeCell ref="Z6:AC6"/>
-    <mergeCell ref="E7:M7"/>
-    <mergeCell ref="N7:U7"/>
-    <mergeCell ref="V7:Y7"/>
-    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="D8:L8"/>
+    <mergeCell ref="D9:L9"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="F11:N11"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="X1:AA1"/>
+    <mergeCell ref="X2:AA2"/>
+    <mergeCell ref="A1:D5"/>
+    <mergeCell ref="M6:T6"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="D6:L6"/>
+    <mergeCell ref="Y7:AB7"/>
+    <mergeCell ref="U6:X6"/>
+    <mergeCell ref="Y6:AB6"/>
+    <mergeCell ref="D7:L7"/>
+    <mergeCell ref="M7:T7"/>
+    <mergeCell ref="U7:X7"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="R16:T16"/>
+    <mergeCell ref="R18:T18"/>
+    <mergeCell ref="F13:N13"/>
+    <mergeCell ref="F14:N14"/>
+    <mergeCell ref="F15:N15"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="F17:N17"/>
+    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="F18:N18"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="C19:E19"/>
+    <mergeCell ref="F19:N19"/>
+    <mergeCell ref="F20:N20"/>
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="F21:N21"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="F12:N12"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="F16:N16"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="R13:T13"/>
+    <mergeCell ref="R12:T12"/>
+    <mergeCell ref="O14:Q14"/>
+    <mergeCell ref="Y20:AB20"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="O12:Q12"/>
+    <mergeCell ref="O13:Q13"/>
+    <mergeCell ref="M8:T8"/>
+    <mergeCell ref="M9:T9"/>
+    <mergeCell ref="Y8:AB8"/>
+    <mergeCell ref="Y9:AB9"/>
+    <mergeCell ref="Y11:AB11"/>
+    <mergeCell ref="U8:X8"/>
+    <mergeCell ref="U9:X9"/>
+    <mergeCell ref="R11:T11"/>
+    <mergeCell ref="U11:X11"/>
+    <mergeCell ref="O11:Q11"/>
+    <mergeCell ref="O16:Q16"/>
+    <mergeCell ref="R17:T17"/>
+    <mergeCell ref="Y25:AB25"/>
+    <mergeCell ref="Y24:AB24"/>
+    <mergeCell ref="Y23:AB23"/>
+    <mergeCell ref="Y22:AB22"/>
+    <mergeCell ref="Y21:AB21"/>
+    <mergeCell ref="U23:X23"/>
+    <mergeCell ref="U24:X24"/>
+    <mergeCell ref="U25:X25"/>
+    <mergeCell ref="Y12:AB12"/>
+    <mergeCell ref="Y13:AB13"/>
+    <mergeCell ref="Y14:AB14"/>
+    <mergeCell ref="Y15:AB15"/>
+    <mergeCell ref="Y16:AB16"/>
+    <mergeCell ref="Y17:AB17"/>
+    <mergeCell ref="Y18:AB18"/>
+    <mergeCell ref="Y19:AB19"/>
+    <mergeCell ref="U26:X26"/>
+    <mergeCell ref="U22:X22"/>
+    <mergeCell ref="O19:Q19"/>
+    <mergeCell ref="O20:Q20"/>
+    <mergeCell ref="O21:Q21"/>
+    <mergeCell ref="A22:T25"/>
+    <mergeCell ref="U21:X21"/>
+    <mergeCell ref="U12:X12"/>
+    <mergeCell ref="U13:X13"/>
+    <mergeCell ref="U14:X14"/>
+    <mergeCell ref="U15:X15"/>
+    <mergeCell ref="U16:X16"/>
+    <mergeCell ref="U17:X17"/>
+    <mergeCell ref="U18:X18"/>
+    <mergeCell ref="U19:X19"/>
+    <mergeCell ref="U20:X20"/>
+    <mergeCell ref="R20:T20"/>
+    <mergeCell ref="R21:T21"/>
+    <mergeCell ref="O15:Q15"/>
+    <mergeCell ref="R14:T14"/>
+    <mergeCell ref="R15:T15"/>
+    <mergeCell ref="O17:Q17"/>
+    <mergeCell ref="O18:Q18"/>
+    <mergeCell ref="R19:T19"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="N9" r:id="rId1" xr:uid="{7BAE6DBD-5FB7-4C97-A379-A5E46272F91D}"/>
+    <hyperlink ref="M9" r:id="rId1" xr:uid="{7BAE6DBD-5FB7-4C97-A379-A5E46272F91D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>